<commit_message>
create auth interceptor but not tested
</commit_message>
<xml_diff>
--- a/docs/v1.0/owl_api.xlsx
+++ b/docs/v1.0/owl_api.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\안덕환\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thekan\workspace\java\OwlAPI\docs\v1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Restful API" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
   <si>
     <t>Title</t>
   </si>
@@ -93,10 +93,6 @@
   <si>
     <t> Create CCTV (CCTV 생성)
  - 개인 당 권한에 따라 할당할 수 있는 CCTV에 제한을 둔다</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> /users/{user id}/cctv</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -166,6 +162,55 @@
   <si>
     <t xml:space="preserve"> - 헤더에 JWT 토큰을 저장한다 (key: "token")
  - 주로 비디오를 보거나 업로드에 사용된다 </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t> Get My All CCTV (내 CCTV 모두 조회하기)
+ - 사용자가 생성한 CCTV의 목록을 모두 가져온다</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> /owners/{user id}/cctvs</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t> GET</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t> - 헤더에 인증 토큰이 있어야 한다</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t> - 헤더에 인증 토큰이 있어야 한다</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> None</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t> Code: 200 Ok
+ Contents: { "msg": "ok", "code": 200, "cctvList": [
+ "cctv": {
+  "description": "", "location": "", "id": ,
+  "registerDate": "", "authCode": "" }}, .. ] }</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> /owners/{user id}/cctvs/{cctv id}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t> Get My CCTV By Id 
+ - 사용자의 CCTV중 ID로 특정 CCTV 정보 조회하기</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t> Code: 200 Ok
+ Contents: { "msg": "ok", "code": 200, "cctv": {
+  "description": "", "location": "",
+  "registerDate": "", "authCode": "" } }</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -316,31 +361,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -662,323 +707,451 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="10.59765625" customWidth="1"/>
     <col min="3" max="3" width="51.8984375" customWidth="1"/>
-    <col min="7" max="7" width="46.09765625" customWidth="1"/>
+    <col min="7" max="7" width="50.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>24</v>
+      <c r="G7" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B8" s="10"/>
-      <c r="C8" s="3"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="3"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>24</v>
+      <c r="G9" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B10" s="10"/>
-      <c r="C10" s="3"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="3"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="6"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>31</v>
+      <c r="G11" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="3"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="6"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>27</v>
+      <c r="G13" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B14" s="7"/>
-      <c r="C14" s="3"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="6"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="2:7" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="B18" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="B18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B19" s="8" t="s">
+      <c r="F18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B21" s="9" t="s">
+      <c r="F20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B22" s="10"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B23" s="9" t="s">
+      <c r="F21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B22" s="8"/>
+      <c r="C22" s="6"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B24" s="10"/>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B25" s="4" t="s">
+      <c r="C23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B25" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B26" s="5"/>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B27" s="6" t="s">
+      <c r="F25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="10"/>
+      <c r="C26" s="6"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="4"/>
+      <c r="C28" s="6"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="B32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="7"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B29" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="B32" s="8" t="s">
+      <c r="F32" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="G32" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B33" s="8" t="s">
+      <c r="F33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B34" s="8" t="s">
+      <c r="G33" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B35" s="9" t="s">
+      <c r="F34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B35" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B37" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B36" s="10"/>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B37" s="9" t="s">
+      <c r="F37" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="G37" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B38" s="8"/>
+      <c r="C38" s="6"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B39" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B38" s="10"/>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B39" s="4" t="s">
+      <c r="F39" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="G39" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="10"/>
+      <c r="C40" s="6"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B40" s="5"/>
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B41" s="6" t="s">
+      <c r="F41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B42" s="7"/>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B43" s="8" t="s">
+      <c r="G41" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B42" s="4"/>
+      <c r="C42" s="6"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B43" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
+  <mergeCells count="48">
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="F7:F8"/>
@@ -995,14 +1168,14 @@
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished the jwt token test
</commit_message>
<xml_diff>
--- a/docs/v1.0/owl_api.xlsx
+++ b/docs/v1.0/owl_api.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Restful API" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>Title</t>
   </si>
@@ -211,6 +211,10 @@
  Contents: { "msg": "ok", "code": 200, "cctv": {
   "description": "", "location": "",
   "registerDate": "", "authCode": "" } }</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> /owners/{user id}/cctvs</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -707,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -879,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.4">
@@ -1128,30 +1132,14 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="F7:F8"/>
@@ -1168,14 +1156,30 @@
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
complete uploading video via azure storage using sas token
</commit_message>
<xml_diff>
--- a/docs/v1.0/owl_api.xlsx
+++ b/docs/v1.0/owl_api.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Restful API" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t>Title</t>
   </si>
@@ -142,16 +142,7 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> /users/{user id}/uploadKey</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t> GET</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t> Get Access Video Key
- - 비디오 액세스에 사용되는 공개키를 받아온다</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -215,6 +206,24 @@
   </si>
   <si>
     <t xml:space="preserve"> /owners/{user id}/cctvs</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t> Get Upload Video Key
+ - 비디오 업로드에 사용될 SAS 키를 받아온다</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> key: video / value: {video name to upload}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> /owner/{user id}/uploadKeys</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t> Code: 400 Bad Request
+ Contents: { "msg": "error message", "code": 401 }</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -711,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -733,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.4">
@@ -747,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.4">
@@ -761,7 +770,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
@@ -775,7 +784,7 @@
         <v>8</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.4">
@@ -815,7 +824,7 @@
         <v>12</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.4">
@@ -835,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.4">
@@ -855,7 +864,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="31.2" x14ac:dyDescent="0.4">
@@ -869,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.4">
@@ -877,13 +886,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.4">
@@ -897,7 +906,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.4">
@@ -931,7 +940,7 @@
         <v>10</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.4">
@@ -951,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.4">
@@ -985,13 +994,13 @@
         <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="31.2" x14ac:dyDescent="0.4">
@@ -1005,7 +1014,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.4">
@@ -1019,7 +1028,7 @@
         <v>2</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.4">
@@ -1033,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.4">
@@ -1067,7 +1076,7 @@
         <v>10</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.4">
@@ -1087,7 +1096,7 @@
         <v>12</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.4">
@@ -1127,19 +1136,35 @@
         <v>4</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="F7:F8"/>
@@ -1156,30 +1181,14 @@
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>